<commit_message>
añado sus y plantilla informe usabilidad
</commit_message>
<xml_diff>
--- a/P4/Cuestionario SUS DIU.xlsx
+++ b/P4/Cuestionario SUS DIU.xlsx
@@ -941,13 +941,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K1007"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.71"/>
@@ -1181,8 +1181,12 @@
         <v>-1</v>
       </c>
       <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
+      <c r="F14" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="30" t="n">
+        <v>2</v>
+      </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
@@ -1201,8 +1205,12 @@
         <v>5</v>
       </c>
       <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
+      <c r="F15" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="30" t="n">
+        <v>3</v>
+      </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
@@ -1221,8 +1229,12 @@
         <v>-1</v>
       </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
+      <c r="F16" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" s="30" t="n">
+        <v>3</v>
+      </c>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
@@ -1241,8 +1253,12 @@
         <v>5</v>
       </c>
       <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
+      <c r="F17" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="30" t="n">
+        <v>2</v>
+      </c>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
@@ -1261,8 +1277,12 @@
         <v>-1</v>
       </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="30"/>
+      <c r="F18" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" s="30" t="n">
+        <v>3</v>
+      </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
@@ -1281,8 +1301,12 @@
         <v>5</v>
       </c>
       <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="30"/>
+      <c r="F19" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G19" s="30" t="n">
+        <v>3</v>
+      </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
@@ -1301,8 +1325,12 @@
         <v>-1</v>
       </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
+      <c r="F20" s="29" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="30" t="n">
+        <v>3</v>
+      </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
@@ -1321,8 +1349,12 @@
         <v>5</v>
       </c>
       <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30"/>
+      <c r="F21" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="30" t="n">
+        <v>2</v>
+      </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
@@ -1341,8 +1373,12 @@
         <v>-1</v>
       </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
+      <c r="F22" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G22" s="30" t="n">
+        <v>2</v>
+      </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
@@ -1361,8 +1397,12 @@
         <v>5</v>
       </c>
       <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
+      <c r="F23" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="30" t="n">
+        <v>1</v>
+      </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
@@ -1387,11 +1427,11 @@
       </c>
       <c r="F24" s="34" t="n">
         <f aca="false">((F14-1)+(5-F15)+(F16-1)+(5-F17)+(F18-1)+(5-F19)+(F20-1)+(5-F21)+(F22-1)+(5-F23))*2.5</f>
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="G24" s="35" t="n">
         <f aca="false">((G14-1)+(5-G15)+(G16-1)+(5-G17)+(G18-1)+(5-G19)+(G20-1)+(5-G21)+(G22-1)+(5-G23))*2.5</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>

</xml_diff>

<commit_message>
añado reseña nuestra aplicacion
</commit_message>
<xml_diff>
--- a/P4/Cuestionario SUS DIU.xlsx
+++ b/P4/Cuestionario SUS DIU.xlsx
@@ -943,11 +943,11 @@
   </sheetPr>
   <dimension ref="A1:K1007"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.71"/>
@@ -1175,12 +1175,16 @@
       <c r="B14" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="D14" s="27" t="n">
         <f aca="false">C14-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E14" s="28"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="28" t="n">
+        <v>2</v>
+      </c>
       <c r="F14" s="29" t="n">
         <v>2</v>
       </c>
@@ -1199,12 +1203,16 @@
       <c r="B15" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="D15" s="27" t="n">
         <f aca="false">5-C15</f>
-        <v>5</v>
-      </c>
-      <c r="E15" s="28"/>
+        <v>4</v>
+      </c>
+      <c r="E15" s="28" t="n">
+        <v>1</v>
+      </c>
       <c r="F15" s="29" t="n">
         <v>1</v>
       </c>
@@ -1223,12 +1231,16 @@
       <c r="B16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="D16" s="27" t="n">
         <f aca="false">C16-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E16" s="28"/>
+        <v>2</v>
+      </c>
+      <c r="E16" s="28" t="n">
+        <v>4</v>
+      </c>
       <c r="F16" s="29" t="n">
         <v>4</v>
       </c>
@@ -1247,12 +1259,16 @@
       <c r="B17" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="26"/>
+      <c r="C17" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="D17" s="27" t="n">
         <f aca="false">5-C17</f>
-        <v>5</v>
-      </c>
-      <c r="E17" s="28"/>
+        <v>3</v>
+      </c>
+      <c r="E17" s="28" t="n">
+        <v>1</v>
+      </c>
       <c r="F17" s="29" t="n">
         <v>1</v>
       </c>
@@ -1271,12 +1287,16 @@
       <c r="B18" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="26"/>
+      <c r="C18" s="26" t="n">
+        <v>4</v>
+      </c>
       <c r="D18" s="27" t="n">
         <f aca="false">C18-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E18" s="28"/>
+        <v>3</v>
+      </c>
+      <c r="E18" s="28" t="n">
+        <v>4</v>
+      </c>
       <c r="F18" s="29" t="n">
         <v>4</v>
       </c>
@@ -1295,12 +1315,16 @@
       <c r="B19" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="D19" s="27" t="n">
         <f aca="false">5-C19</f>
-        <v>5</v>
-      </c>
-      <c r="E19" s="28"/>
+        <v>3</v>
+      </c>
+      <c r="E19" s="28" t="n">
+        <v>2</v>
+      </c>
       <c r="F19" s="29" t="n">
         <v>3</v>
       </c>
@@ -1319,12 +1343,16 @@
       <c r="B20" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="D20" s="27" t="n">
         <f aca="false">C20-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E20" s="28"/>
+        <v>2</v>
+      </c>
+      <c r="E20" s="28" t="n">
+        <v>4</v>
+      </c>
       <c r="F20" s="29" t="n">
         <v>5</v>
       </c>
@@ -1343,12 +1371,16 @@
       <c r="B21" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="D21" s="27" t="n">
         <f aca="false">5-C21</f>
-        <v>5</v>
-      </c>
-      <c r="E21" s="28"/>
+        <v>4</v>
+      </c>
+      <c r="E21" s="28" t="n">
+        <v>1</v>
+      </c>
       <c r="F21" s="29" t="n">
         <v>2</v>
       </c>
@@ -1367,12 +1399,16 @@
       <c r="B22" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="26"/>
+      <c r="C22" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="D22" s="27" t="n">
         <f aca="false">C22-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E22" s="28"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="28" t="n">
+        <v>4</v>
+      </c>
       <c r="F22" s="29" t="n">
         <v>3</v>
       </c>
@@ -1391,12 +1427,16 @@
       <c r="B23" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="26" t="n">
+        <v>1</v>
+      </c>
       <c r="D23" s="27" t="n">
         <f aca="false">5-C23</f>
-        <v>5</v>
-      </c>
-      <c r="E23" s="28"/>
+        <v>4</v>
+      </c>
+      <c r="E23" s="28" t="n">
+        <v>1</v>
+      </c>
       <c r="F23" s="29" t="n">
         <v>1</v>
       </c>
@@ -1415,15 +1455,15 @@
       </c>
       <c r="C24" s="31" t="n">
         <f aca="false">((C14-1)+(5-C15)+(C16-1)+(5-C17)+(C18-1)+(5-C19)+(C20-1)+(5-C21)+(C22-1)+(5-C23))*2.5</f>
-        <v>50</v>
+        <v>67.5</v>
       </c>
       <c r="D24" s="32" t="n">
         <f aca="false">(SUM(D14:D23))*2.5</f>
-        <v>50</v>
+        <v>67.5</v>
       </c>
       <c r="E24" s="33" t="n">
         <f aca="false">((E14-1)+(5-E15)+(E16-1)+(5-E17)+(E18-1)+(5-E19)+(E20-1)+(5-E21)+(E22-1)+(5-E23))*2.5</f>
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F24" s="34" t="n">
         <f aca="false">((F14-1)+(5-F15)+(F16-1)+(5-F17)+(F18-1)+(5-F19)+(F20-1)+(5-F21)+(F22-1)+(5-F23))*2.5</f>

</xml_diff>

<commit_message>
Acabo practica se supone2
</commit_message>
<xml_diff>
--- a/P4/Cuestionario SUS DIU.xlsx
+++ b/P4/Cuestionario SUS DIU.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t xml:space="preserve">EQUIPO:                                           (fecha)</t>
   </si>
@@ -76,40 +76,37 @@
     <t xml:space="preserve">OCUPACION</t>
   </si>
   <si>
-    <t xml:space="preserve">Profesor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arquitecta</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estudiante</t>
   </si>
   <si>
+    <t xml:space="preserve">Ama de casa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Físico</t>
+  </si>
+  <si>
     <t xml:space="preserve">EXPERIENCIA TIC</t>
   </si>
   <si>
+    <t xml:space="preserve">Alta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baja</t>
   </si>
   <si>
-    <t xml:space="preserve">Alta</t>
-  </si>
-  <si>
     <t xml:space="preserve">PERFIL (describir)</t>
   </si>
   <si>
-    <t xml:space="preserve">4,4,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,1,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,6,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,5,2</t>
+    <t xml:space="preserve">Estudiante tranquilo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ama de casa feliz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trabajador tranquilo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudiante enfadada</t>
   </si>
   <si>
     <t xml:space="preserve">1: Completamente en desacuerdo</t>
@@ -943,11 +940,11 @@
   </sheetPr>
   <dimension ref="A1:K1007"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.71"/>
@@ -1025,10 +1022,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1036,17 +1033,17 @@
         <v>16</v>
       </c>
       <c r="C6" s="8" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6" s="12" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G6" s="11" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1064,22 +1061,22 @@
         <v>20</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>23</v>
@@ -1087,20 +1084,20 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1112,31 +1109,31 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C11" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C12" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -1146,22 +1143,22 @@
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18"/>
       <c r="B13" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="D13" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="E13" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="22" t="s">
-        <v>36</v>
-      </c>
       <c r="G13" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
@@ -1173,23 +1170,23 @@
         <v>1</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="26" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14" s="27" t="n">
         <f aca="false">C14-1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14" s="28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="29" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G14" s="30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
@@ -1201,7 +1198,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="26" t="n">
         <v>1</v>
@@ -1214,10 +1211,10 @@
         <v>1</v>
       </c>
       <c r="F15" s="29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
@@ -1229,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="26" t="n">
         <v>3</v>
@@ -1242,10 +1239,10 @@
         <v>4</v>
       </c>
       <c r="F16" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="30" t="n">
         <v>4</v>
-      </c>
-      <c r="G16" s="30" t="n">
-        <v>3</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
@@ -1257,23 +1254,23 @@
         <v>4</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="27" t="n">
         <f aca="false">5-C17</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="30" t="n">
         <v>1</v>
-      </c>
-      <c r="F17" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="30" t="n">
-        <v>2</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
@@ -1285,7 +1282,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="26" t="n">
         <v>4</v>
@@ -1298,10 +1295,10 @@
         <v>4</v>
       </c>
       <c r="F18" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="30" t="n">
         <v>4</v>
-      </c>
-      <c r="G18" s="30" t="n">
-        <v>3</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
@@ -1313,7 +1310,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="26" t="n">
         <v>2</v>
@@ -1326,7 +1323,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G19" s="30" t="n">
         <v>3</v>
@@ -1341,7 +1338,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="26" t="n">
         <v>3</v>
@@ -1351,13 +1348,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="28" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="30" t="n">
         <v>4</v>
-      </c>
-      <c r="F20" s="29" t="n">
-        <v>5</v>
-      </c>
-      <c r="G20" s="30" t="n">
-        <v>3</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
@@ -1369,23 +1366,23 @@
         <v>8</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="27" t="n">
         <f aca="false">5-C21</f>
+        <v>3</v>
+      </c>
+      <c r="E21" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="30" t="n">
         <v>4</v>
-      </c>
-      <c r="E21" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="30" t="n">
-        <v>2</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
@@ -1397,14 +1394,14 @@
         <v>9</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="26" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D22" s="27" t="n">
         <f aca="false">C22-1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22" s="28" t="n">
         <v>4</v>
@@ -1413,7 +1410,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
@@ -1425,7 +1422,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="26" t="n">
         <v>1</v>
@@ -1438,10 +1435,10 @@
         <v>1</v>
       </c>
       <c r="F23" s="29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
@@ -1451,15 +1448,15 @@
     <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="17"/>
       <c r="B24" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="31" t="n">
         <f aca="false">((C14-1)+(5-C15)+(C16-1)+(5-C17)+(C18-1)+(5-C19)+(C20-1)+(5-C21)+(C22-1)+(5-C23))*2.5</f>
-        <v>67.5</v>
+        <v>77.5</v>
       </c>
       <c r="D24" s="32" t="n">
         <f aca="false">(SUM(D14:D23))*2.5</f>
-        <v>67.5</v>
+        <v>77.5</v>
       </c>
       <c r="E24" s="33" t="n">
         <f aca="false">((E14-1)+(5-E15)+(E16-1)+(5-E17)+(E18-1)+(5-E19)+(E20-1)+(5-E21)+(E22-1)+(5-E23))*2.5</f>
@@ -1467,11 +1464,11 @@
       </c>
       <c r="F24" s="34" t="n">
         <f aca="false">((F14-1)+(5-F15)+(F16-1)+(5-F17)+(F18-1)+(5-F19)+(F20-1)+(5-F21)+(F22-1)+(5-F23))*2.5</f>
-        <v>75</v>
+        <v>67.5</v>
       </c>
       <c r="G24" s="35" t="n">
         <f aca="false">((G14-1)+(5-G15)+(G16-1)+(5-G17)+(G18-1)+(5-G19)+(G20-1)+(5-G21)+(G22-1)+(5-G23))*2.5</f>
-        <v>55</v>
+        <v>67.5</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
@@ -1480,44 +1477,44 @@
     </row>
     <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="37"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="37"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Añado readme y cambios menores
</commit_message>
<xml_diff>
--- a/P4/Cuestionario SUS DIU.xlsx
+++ b/P4/Cuestionario SUS DIU.xlsx
@@ -20,21 +20,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
-  <si>
-    <t xml:space="preserve">EQUIPO:                                           (fecha)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST A:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST B:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+  <si>
+    <t xml:space="preserve">EQUIPO: DIU2.Marmotas          23/05/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST A: DIU2.Marmotas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST B: DIU1.Lex</t>
   </si>
   <si>
     <t xml:space="preserve">DISEÑO DE INTERFACES DE USUARIO </t>
   </si>
   <si>
-    <t xml:space="preserve">Web: </t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Web:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://github.com/Mapachana/DIU21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Web: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://github.com/lawvp/DIU21</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">PRACTICA 4 - Cuestionario SUS </t>
@@ -384,7 +423,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -416,6 +455,13 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
@@ -728,7 +774,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -736,35 +782,35 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -776,7 +822,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -792,51 +838,51 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -848,7 +894,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -940,17 +986,19 @@
   </sheetPr>
   <dimension ref="A1:K1007"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.59"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="27.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="27.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.01"/>
   </cols>
   <sheetData>
@@ -974,63 +1022,63 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="8" t="n">
         <v>23</v>
@@ -1048,56 +1096,56 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>22</v>
-      </c>
       <c r="G8" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1109,31 +1157,31 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C11" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C12" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -1143,22 +1191,22 @@
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18"/>
       <c r="B13" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
@@ -1170,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="26" t="n">
         <v>4</v>
@@ -1198,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="26" t="n">
         <v>1</v>
@@ -1226,7 +1274,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="26" t="n">
         <v>3</v>
@@ -1254,7 +1302,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" s="26" t="n">
         <v>1</v>
@@ -1282,7 +1330,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" s="26" t="n">
         <v>4</v>
@@ -1310,7 +1358,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="26" t="n">
         <v>2</v>
@@ -1338,7 +1386,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="26" t="n">
         <v>3</v>
@@ -1366,7 +1414,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="26" t="n">
         <v>2</v>
@@ -1394,7 +1442,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="26" t="n">
         <v>4</v>
@@ -1422,7 +1470,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" s="26" t="n">
         <v>1</v>
@@ -1448,7 +1496,7 @@
     <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="17"/>
       <c r="B24" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" s="31" t="n">
         <f aca="false">((C14-1)+(5-C15)+(C16-1)+(5-C17)+(C18-1)+(5-C19)+(C20-1)+(5-C21)+(C22-1)+(5-C23))*2.5</f>
@@ -1477,44 +1525,44 @@
     </row>
     <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C25" s="37"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26" s="37"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2503,7 +2551,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B34" r:id="rId1" display="http://www.measuringux.com/sus/SUS.pdf"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://github.com/Mapachana/DIU21"/>
+    <hyperlink ref="F2" r:id="rId2" display="https://github.com/lawvp/DIU21"/>
+    <hyperlink ref="B34" r:id="rId3" display="http://www.measuringux.com/sus/SUS.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Cambio conclusiones y correcciones menores
</commit_message>
<xml_diff>
--- a/P4/Cuestionario SUS DIU.xlsx
+++ b/P4/Cuestionario SUS DIU.xlsx
@@ -34,46 +34,10 @@
     <t xml:space="preserve">DISEÑO DE INTERFACES DE USUARIO </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Web:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/Mapachana/DIU21</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Web: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/lawvp/DIU21</t>
-    </r>
+    <t xml:space="preserve">Web:  https://github.com/Mapachana/DIU21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web: https://github.com/lawvp/DIU21</t>
   </si>
   <si>
     <t xml:space="preserve">PRACTICA 4 - Cuestionario SUS </t>
@@ -136,16 +100,16 @@
     <t xml:space="preserve">PERFIL (describir)</t>
   </si>
   <si>
-    <t xml:space="preserve">Estudiante tranquilo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ama de casa feliz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trabajador tranquilo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudiante enfadada</t>
+    <t xml:space="preserve">Introvertido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extrovertida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Racional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introvertida</t>
   </si>
   <si>
     <t xml:space="preserve">1: Completamente en desacuerdo</t>
@@ -741,7 +705,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -751,6 +715,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -987,17 +955,17 @@
   <dimension ref="A1:K1007"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.59"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="27.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.01"/>
   </cols>
@@ -1018,10 +986,10 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1030,528 +998,528 @@
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C6" s="9" t="n">
         <v>23</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10" t="n">
+      <c r="D6" s="10"/>
+      <c r="E6" s="11" t="n">
         <v>57</v>
       </c>
-      <c r="F6" s="12" t="n">
+      <c r="F6" s="13" t="n">
         <v>26</v>
       </c>
-      <c r="G6" s="11" t="n">
+      <c r="G6" s="12" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="7"/>
-      <c r="C10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="n">
+      <c r="A14" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="26" t="n">
+      <c r="C14" s="27" t="n">
         <v>4</v>
       </c>
-      <c r="D14" s="27" t="n">
+      <c r="D14" s="28" t="n">
         <f aca="false">C14-1</f>
         <v>3</v>
       </c>
-      <c r="E14" s="28" t="n">
+      <c r="E14" s="29" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="29" t="n">
+      <c r="F14" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="G14" s="30" t="n">
+      <c r="G14" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="n">
+      <c r="A15" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="26" t="n">
+      <c r="C15" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="27" t="n">
+      <c r="D15" s="28" t="n">
         <f aca="false">5-C15</f>
         <v>4</v>
       </c>
-      <c r="E15" s="28" t="n">
+      <c r="E15" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="29" t="n">
+      <c r="F15" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="G15" s="30" t="n">
+      <c r="G15" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="n">
+      <c r="A16" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="26" t="n">
+      <c r="C16" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="D16" s="27" t="n">
+      <c r="D16" s="28" t="n">
         <f aca="false">C16-1</f>
         <v>2</v>
       </c>
-      <c r="E16" s="28" t="n">
+      <c r="E16" s="29" t="n">
         <v>4</v>
       </c>
-      <c r="F16" s="29" t="n">
+      <c r="F16" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="30" t="n">
+      <c r="G16" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="n">
+      <c r="A17" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="26" t="n">
+      <c r="C17" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="27" t="n">
+      <c r="D17" s="28" t="n">
         <f aca="false">5-C17</f>
         <v>4</v>
       </c>
-      <c r="E17" s="28" t="n">
+      <c r="E17" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="29" t="n">
+      <c r="F17" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="30" t="n">
+      <c r="G17" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="n">
+      <c r="A18" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="26" t="n">
+      <c r="C18" s="27" t="n">
         <v>4</v>
       </c>
-      <c r="D18" s="27" t="n">
+      <c r="D18" s="28" t="n">
         <f aca="false">C18-1</f>
         <v>3</v>
       </c>
-      <c r="E18" s="28" t="n">
+      <c r="E18" s="29" t="n">
         <v>4</v>
       </c>
-      <c r="F18" s="29" t="n">
+      <c r="F18" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="G18" s="30" t="n">
+      <c r="G18" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="n">
+      <c r="A19" s="25" t="n">
         <v>6</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="26" t="n">
+      <c r="C19" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="D19" s="27" t="n">
+      <c r="D19" s="28" t="n">
         <f aca="false">5-C19</f>
         <v>3</v>
       </c>
-      <c r="E19" s="28" t="n">
+      <c r="E19" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="F19" s="29" t="n">
+      <c r="F19" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="30" t="n">
+      <c r="G19" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="n">
+      <c r="A20" s="25" t="n">
         <v>7</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="26" t="n">
+      <c r="C20" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="D20" s="27" t="n">
+      <c r="D20" s="28" t="n">
         <f aca="false">C20-1</f>
         <v>2</v>
       </c>
-      <c r="E20" s="28" t="n">
+      <c r="E20" s="29" t="n">
         <v>5</v>
       </c>
-      <c r="F20" s="29" t="n">
+      <c r="F20" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="G20" s="30" t="n">
+      <c r="G20" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
     </row>
     <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="n">
+      <c r="A21" s="25" t="n">
         <v>8</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="26" t="n">
+      <c r="C21" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="27" t="n">
+      <c r="D21" s="28" t="n">
         <f aca="false">5-C21</f>
         <v>3</v>
       </c>
-      <c r="E21" s="28" t="n">
+      <c r="E21" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="F21" s="29" t="n">
+      <c r="F21" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="30" t="n">
+      <c r="G21" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="n">
+      <c r="A22" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="26" t="n">
+      <c r="C22" s="27" t="n">
         <v>4</v>
       </c>
-      <c r="D22" s="27" t="n">
+      <c r="D22" s="28" t="n">
         <f aca="false">C22-1</f>
         <v>3</v>
       </c>
-      <c r="E22" s="28" t="n">
+      <c r="E22" s="29" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="29" t="n">
+      <c r="F22" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="30" t="n">
+      <c r="G22" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
     </row>
     <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24" t="n">
+      <c r="A23" s="25" t="n">
         <v>10</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="26" t="n">
+      <c r="C23" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="27" t="n">
+      <c r="D23" s="28" t="n">
         <f aca="false">5-C23</f>
         <v>4</v>
       </c>
-      <c r="E23" s="28" t="n">
+      <c r="E23" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="29" t="n">
+      <c r="F23" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="G23" s="30" t="n">
+      <c r="G23" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
     </row>
     <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17"/>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="31" t="n">
+      <c r="C24" s="32" t="n">
         <f aca="false">((C14-1)+(5-C15)+(C16-1)+(5-C17)+(C18-1)+(5-C19)+(C20-1)+(5-C21)+(C22-1)+(5-C23))*2.5</f>
         <v>77.5</v>
       </c>
-      <c r="D24" s="32" t="n">
+      <c r="D24" s="33" t="n">
         <f aca="false">(SUM(D14:D23))*2.5</f>
         <v>77.5</v>
       </c>
-      <c r="E24" s="33" t="n">
+      <c r="E24" s="34" t="n">
         <f aca="false">((E14-1)+(5-E15)+(E16-1)+(5-E17)+(E18-1)+(5-E19)+(E20-1)+(5-E21)+(E22-1)+(5-E23))*2.5</f>
         <v>80</v>
       </c>
-      <c r="F24" s="34" t="n">
+      <c r="F24" s="35" t="n">
         <f aca="false">((F14-1)+(5-F15)+(F16-1)+(5-F17)+(F18-1)+(5-F19)+(F20-1)+(5-F21)+(F22-1)+(5-F23))*2.5</f>
         <v>67.5</v>
       </c>
-      <c r="G24" s="35" t="n">
+      <c r="G24" s="36" t="n">
         <f aca="false">((G14-1)+(5-G15)+(G16-1)+(5-G17)+(G18-1)+(5-G19)+(G20-1)+(5-G21)+(G22-1)+(5-G23))*2.5</f>
         <v>67.5</v>
       </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
     </row>
     <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="37"/>
+      <c r="C25" s="38"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="37"/>
+      <c r="C26" s="38"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1561,7 +1529,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="39" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2551,8 +2519,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://github.com/Mapachana/DIU21"/>
-    <hyperlink ref="F2" r:id="rId2" display="https://github.com/lawvp/DIU21"/>
+    <hyperlink ref="C2" r:id="rId1" display="Web:  https://github.com/Mapachana/DIU21"/>
+    <hyperlink ref="F2" r:id="rId2" display="Web: https://github.com/lawvp/DIU21"/>
     <hyperlink ref="B34" r:id="rId3" display="http://www.measuringux.com/sus/SUS.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>

</xml_diff>